<commit_message>
updated Dataschema_TRACY to include "don't know" in family history variables
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_schema/Dataschema_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_schema/Dataschema_TRACY.xlsx
@@ -1407,7 +1407,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2018,16 +2018,16 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>FAM1_DIAB2</t>
+          <t>FAM1_CHD_STROKE</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>don't know</t>
         </is>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -2038,26 +2038,26 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>FAM1_CANCER</t>
+          <t>FAM1_DIAB2</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -2068,47 +2068,47 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>DRE_SCREEN</t>
+          <t>FAM1_CANCER</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>DRE_SCREEN</t>
+          <t>FAM1_CANCER</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>don't know</t>
         </is>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>PSA_SCREEN</t>
+          <t>DRE_SCREEN</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2123,7 +2123,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PSA_SCREEN</t>
+          <t>DRE_SCREEN</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>FOBT_SCREEN</t>
+          <t>PSA_SCREEN</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2153,7 +2153,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>FOBT_SCREEN</t>
+          <t>PSA_SCREEN</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2168,7 +2168,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>COL_SCREEN</t>
+          <t>FOBT_SCREEN</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2183,7 +2183,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>COL_SCREEN</t>
+          <t>FOBT_SCREEN</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2198,7 +2198,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MELANOMA_SCREEN</t>
+          <t>COL_SCREEN</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2213,7 +2213,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>MELANOMA_SCREEN</t>
+          <t>COL_SCREEN</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>MAMMO_SCREEN</t>
+          <t>MELANOMA_SCREEN</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>MAMMO_SCREEN</t>
+          <t>MELANOMA_SCREEN</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2258,7 +2258,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CERVICAL_SCREEN</t>
+          <t>MAMMO_SCREEN</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2273,7 +2273,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>CERVICAL_SCREEN</t>
+          <t>MAMMO_SCREEN</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2288,7 +2288,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>MED_STAT</t>
+          <t>CERVICAL_SCREEN</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2303,7 +2303,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>MED_STAT</t>
+          <t>CERVICAL_SCREEN</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2318,7 +2318,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MED_NSAID</t>
+          <t>MED_STAT</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2333,7 +2333,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MED_NSAID</t>
+          <t>MED_STAT</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2348,7 +2348,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>INC_CVD</t>
+          <t>MED_NSAID</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2363,7 +2363,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>INC_CVD</t>
+          <t>MED_NSAID</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2378,7 +2378,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>INC_ANGINA</t>
+          <t>INC_CVD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2393,7 +2393,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>INC_ANGINA</t>
+          <t>INC_CVD</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>INC_MI</t>
+          <t>INC_ANGINA</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2423,7 +2423,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>INC_MI</t>
+          <t>INC_ANGINA</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2438,7 +2438,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>INC_STR</t>
+          <t>INC_MI</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2453,7 +2453,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>INC_STR</t>
+          <t>INC_MI</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2468,7 +2468,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>INC_ISC_STR</t>
+          <t>INC_STR</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2483,7 +2483,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>INC_ISC_STR</t>
+          <t>INC_STR</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>INC_HAEMO_STR</t>
+          <t>INC_ISC_STR</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2513,7 +2513,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>INC_HAEMO_STR</t>
+          <t>INC_ISC_STR</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2528,7 +2528,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>INC_HYP</t>
+          <t>INC_HAEMO_STR</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2543,7 +2543,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>INC_HYP</t>
+          <t>INC_HAEMO_STR</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2558,7 +2558,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>INC_HF</t>
+          <t>INC_HYP</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2573,7 +2573,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>INC_HF</t>
+          <t>INC_HYP</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2588,7 +2588,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>INC_DIAB2</t>
+          <t>INC_HF</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2603,7 +2603,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>INC_DIAB2</t>
+          <t>INC_HF</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2618,7 +2618,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>INC_CANCER</t>
+          <t>INC_DIAB2</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2633,7 +2633,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>INC_CANCER</t>
+          <t>INC_DIAB2</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2648,7 +2648,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>VITAL_ST</t>
+          <t>INC_CANCER</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2663,7 +2663,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>VITAL_ST</t>
+          <t>INC_CANCER</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2678,7 +2678,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>VITAL_ST_CVD</t>
+          <t>VITAL_ST</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2693,7 +2693,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>VITAL_ST_CVD</t>
+          <t>VITAL_ST</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2708,7 +2708,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>VITAL_ST_CANCER</t>
+          <t>VITAL_ST_CVD</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2723,15 +2723,45 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>VITAL_ST_CVD</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
           <t>VITAL_ST_CANCER</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="C88">
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>VITAL_ST_CANCER</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C90">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated dataschema_p2 and dataschema_tracy to include "I don't know" for family history vars
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_schema/Dataschema_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_schema/Dataschema_TRACY.xlsx
@@ -2023,7 +2023,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>don't know</t>
+          <t>I don't know</t>
         </is>
       </c>
       <c r="C41">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>don't know</t>
+          <t>I don't know</t>
         </is>
       </c>
       <c r="C46">

</xml_diff>